<commit_message>
Got opcode simulation running.
</commit_message>
<xml_diff>
--- a/Architecture/OpCodes/R32V2020.xlsx
+++ b/Architecture/OpCodes/R32V2020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="OpCodes" sheetId="1" state="visible" r:id="rId2"/>
@@ -456,7 +456,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -481,10 +481,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -504,19 +500,20 @@
   </sheetPr>
   <dimension ref="A1:AI42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK10" activeCellId="0" sqref="AK10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="4" style="1" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="21" style="1" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="26" style="1" width="2.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="36" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4516,25 +4513,26 @@
   </sheetPr>
   <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Z11" activeCellId="0" sqref="Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="2" style="0" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="24" style="0" width="2.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="34" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="n">
@@ -4719,7 +4717,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Working on ALU simulation
</commit_message>
<xml_diff>
--- a/Architecture/OpCodes/R32V2020.xlsx
+++ b/Architecture/OpCodes/R32V2020.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="OpCodes" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="CCR" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Resources" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="122">
   <si>
     <t xml:space="preserve">R32V2020 Opcodes</t>
   </si>
@@ -90,9 +90,6 @@
     <t xml:space="preserve">CMP</t>
   </si>
   <si>
-    <t xml:space="preserve">r3</t>
-  </si>
-  <si>
     <t xml:space="preserve">OR 2 regs and store in 3rd</t>
   </si>
   <si>
@@ -358,6 +355,39 @@
   </si>
   <si>
     <t xml:space="preserve">Data Ptr Overflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R32V2020 Resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L.E.s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multipliers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLLs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpCodeDecoder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUX_16x32</t>
   </si>
 </sst>
 </file>
@@ -456,7 +486,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -481,6 +511,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -501,14 +535,14 @@
   <dimension ref="A1:AI42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="4" style="1" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="21" style="1" width="3.79"/>
@@ -1163,7 +1197,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
@@ -1222,10 +1256,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="D9" s="4" t="n">
         <v>0</v>
@@ -1311,10 +1345,10 @@
         <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="D10" s="4" t="n">
         <v>0</v>
@@ -1400,10 +1434,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="4" t="n">
         <v>0</v>
@@ -1489,10 +1523,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="D12" s="4" t="n">
         <v>0</v>
@@ -1525,7 +1559,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
@@ -1578,10 +1612,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="D13" s="4" t="n">
         <v>0</v>
@@ -1614,7 +1648,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
@@ -1667,10 +1701,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D14" s="4" t="n">
         <v>0</v>
@@ -1703,7 +1737,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
@@ -1756,10 +1790,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="D15" s="4" t="n">
         <v>0</v>
@@ -1792,7 +1826,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
@@ -1845,10 +1879,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="D16" s="4" t="n">
         <v>0</v>
@@ -1881,7 +1915,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
@@ -1934,10 +1968,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="D17" s="4" t="n">
         <v>0</v>
@@ -2026,13 +2060,13 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="D18" s="4" t="n">
         <v>0</v>
@@ -2077,7 +2111,7 @@
         <v>7</v>
       </c>
       <c r="T18" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
@@ -2097,13 +2131,13 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="D19" s="4" t="n">
         <v>0</v>
@@ -2148,7 +2182,7 @@
         <v>7</v>
       </c>
       <c r="T19" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U19" s="5"/>
       <c r="V19" s="5"/>
@@ -2168,13 +2202,13 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="D20" s="4" t="n">
         <v>0</v>
@@ -2219,7 +2253,7 @@
         <v>7</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U20" s="5"/>
       <c r="V20" s="5"/>
@@ -2263,14 +2297,14 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="D21" s="4" t="n">
         <v>0</v>
       </c>
@@ -2296,7 +2330,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M21" s="5" t="s">
         <v>7</v>
@@ -2364,13 +2398,13 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="D22" s="4" t="n">
         <v>0</v>
@@ -2415,7 +2449,7 @@
         <v>7</v>
       </c>
       <c r="T22" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U22" s="5"/>
       <c r="V22" s="5"/>
@@ -2459,14 +2493,14 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="D23" s="4" t="n">
         <v>0</v>
       </c>
@@ -2492,7 +2526,7 @@
         <v>1</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
@@ -2554,13 +2588,13 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="D24" s="4" t="n">
         <v>0</v>
@@ -2605,7 +2639,7 @@
         <v>7</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U24" s="5"/>
       <c r="V24" s="5"/>
@@ -2649,14 +2683,14 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="D25" s="4" t="n">
         <v>0</v>
       </c>
@@ -2682,7 +2716,7 @@
         <v>1</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
@@ -2744,13 +2778,13 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="D26" s="4" t="n">
         <v>1</v>
@@ -2795,7 +2829,7 @@
         <v>7</v>
       </c>
       <c r="T26" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U26" s="5"/>
       <c r="V26" s="5"/>
@@ -2839,14 +2873,14 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="D27" s="4" t="n">
         <v>1</v>
       </c>
@@ -2872,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
@@ -2934,13 +2968,13 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="D28" s="4" t="n">
         <v>1</v>
@@ -2985,7 +3019,7 @@
         <v>7</v>
       </c>
       <c r="T28" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U28" s="5"/>
       <c r="V28" s="5"/>
@@ -3029,14 +3063,14 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="D29" s="4" t="n">
         <v>1</v>
       </c>
@@ -3062,7 +3096,7 @@
         <v>1</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
@@ -3124,13 +3158,13 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="D30" s="4" t="n">
         <v>1</v>
@@ -3175,7 +3209,7 @@
         <v>7</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U30" s="5"/>
       <c r="V30" s="5"/>
@@ -3219,14 +3253,14 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="D31" s="4" t="n">
         <v>1</v>
       </c>
@@ -3252,7 +3286,7 @@
         <v>1</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
@@ -3314,40 +3348,40 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="D32" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E32" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G32" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I32" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
@@ -3409,13 +3443,13 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="D33" s="4" t="n">
         <v>1</v>
@@ -3460,7 +3494,7 @@
         <v>7</v>
       </c>
       <c r="T33" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U33" s="5"/>
       <c r="V33" s="5"/>
@@ -3504,40 +3538,40 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D34" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="D34" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E34" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H34" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I34" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J34" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="M34" s="5" t="s">
         <v>7</v>
@@ -3605,13 +3639,13 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="D35" s="4" t="n">
         <v>1</v>
@@ -3712,64 +3746,64 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="D36" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="P36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="S36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="T36" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="D36" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E36" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F36" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I36" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J36" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K36" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="O36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="P36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="R36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="S36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="T36" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="U36" s="4"/>
       <c r="V36" s="4"/>
@@ -3813,14 +3847,14 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="D37" s="4" t="n">
         <v>1</v>
       </c>
@@ -3870,7 +3904,7 @@
         <v>7</v>
       </c>
       <c r="T37" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U37" s="4"/>
       <c r="V37" s="4"/>
@@ -3914,14 +3948,14 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="D38" s="4" t="n">
         <v>1</v>
       </c>
@@ -3971,7 +4005,7 @@
         <v>7</v>
       </c>
       <c r="T38" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U38" s="4"/>
       <c r="V38" s="4"/>
@@ -4015,14 +4049,14 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="D39" s="4" t="n">
         <v>1</v>
       </c>
@@ -4072,7 +4106,7 @@
         <v>7</v>
       </c>
       <c r="T39" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U39" s="4"/>
       <c r="V39" s="4"/>
@@ -4116,14 +4150,14 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="D40" s="4" t="n">
         <v>1</v>
       </c>
@@ -4173,7 +4207,7 @@
         <v>7</v>
       </c>
       <c r="T40" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U40" s="4"/>
       <c r="V40" s="4"/>
@@ -4217,14 +4251,14 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="D41" s="4" t="n">
         <v>1</v>
       </c>
@@ -4274,7 +4308,7 @@
         <v>7</v>
       </c>
       <c r="T41" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U41" s="4"/>
       <c r="V41" s="4"/>
@@ -4318,14 +4352,14 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B42" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="D42" s="4" t="n">
         <v>1</v>
       </c>
@@ -4375,7 +4409,7 @@
         <v>7</v>
       </c>
       <c r="T42" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U42" s="4" t="s">
         <v>7</v>
@@ -4519,7 +4553,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="2" style="0" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="24" style="0" width="2.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="34" style="0" width="8.67"/>
@@ -4527,7 +4561,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4634,7 +4668,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AG4" s="0" t="n">
         <v>1</v>
@@ -4642,7 +4676,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AF5" s="0" t="n">
         <v>1</v>
@@ -4650,7 +4684,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AE6" s="0" t="n">
         <v>1</v>
@@ -4658,7 +4692,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD7" s="0" t="n">
         <v>1</v>
@@ -4666,7 +4700,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AC8" s="0" t="n">
         <v>1</v>
@@ -4674,7 +4708,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AB9" s="0" t="n">
         <v>1</v>
@@ -4682,7 +4716,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AA10" s="0" t="n">
         <v>1</v>
@@ -4690,7 +4724,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Z11" s="0" t="n">
         <v>1</v>
@@ -4715,17 +4749,173 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.71"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>54</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>189</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>594</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>416</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>321</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>416</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="n">
+        <f aca="false">SUM(B3:B10)</f>
+        <v>1158</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <f aca="false">SUM(C3:C10)</f>
+        <v>832</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">SUM(D3:D10)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <f aca="false">SUM(E3:E10)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <f aca="false">SUM(F3:F10)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Greatly simplify ALL branch operations
</commit_message>
<xml_diff>
--- a/Architecture/OpCodes/R32V2020.xlsx
+++ b/Architecture/OpCodes/R32V2020.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="124">
   <si>
     <t xml:space="preserve">R32V2020 Opcodes</t>
   </si>
@@ -285,34 +285,13 @@
     <t xml:space="preserve">Flow_Ctrl</t>
   </si>
   <si>
-    <t xml:space="preserve">Jump to subroutine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JSR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(r7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return from subroutine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JMP</t>
-  </si>
-  <si>
     <t xml:space="preserve">Branch Always</t>
   </si>
   <si>
     <t xml:space="preserve">BRA</t>
   </si>
   <si>
-    <t xml:space="preserve">(rX)</t>
+    <t xml:space="preserve">Relative Address</t>
   </si>
   <si>
     <t xml:space="preserve">Branch if carry is set</t>
@@ -339,10 +318,16 @@
     <t xml:space="preserve">BE1</t>
   </si>
   <si>
-    <t xml:space="preserve">Branch Overflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOV</t>
+    <t xml:space="preserve">Branch Greater Than</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BGT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch Less Than</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLE</t>
   </si>
   <si>
     <t xml:space="preserve">Branch Equal</t>
@@ -418,7 +403,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -457,6 +442,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -466,7 +457,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="34">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -705,34 +696,6 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="hair"/>
-      <top/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -759,7 +722,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -956,32 +919,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1009,10 +948,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI45"/>
+  <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42:K43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L36" activeCellId="0" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4204,107 +4143,107 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="C36" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="E36" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="F36" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I36" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J36" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K36" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L36" s="53" t="s">
+      <c r="D36" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="M36" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="N36" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="O36" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="P36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="R36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="S36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="T36" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="U36" s="54"/>
-      <c r="V36" s="54"/>
-      <c r="W36" s="54"/>
-      <c r="X36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH36" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI36" s="52" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="N36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="O36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="P36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="R36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="S36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="T36" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="U36" s="49"/>
+      <c r="V36" s="49"/>
+      <c r="W36" s="49"/>
+      <c r="X36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI36" s="49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="s">
         <v>86</v>
       </c>
@@ -4338,80 +4277,74 @@
       <c r="K37" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="L37" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="M37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="N37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="O37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="P37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="R37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="S37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="T37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="U37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="V37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="W37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="X37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI37" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L37" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="M37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="N37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="O37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="P37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="R37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="S37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="T37" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="U37" s="49"/>
+      <c r="V37" s="49"/>
+      <c r="W37" s="49"/>
+      <c r="X37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI37" s="49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="12" t="s">
         <v>86</v>
       </c>
@@ -4445,68 +4378,74 @@
       <c r="K38" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="L38" s="42" t="s">
+      <c r="L38" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="M38" s="42"/>
-      <c r="N38" s="42"/>
-      <c r="O38" s="42"/>
-      <c r="P38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="R38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="S38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="T38" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="U38" s="42"/>
-      <c r="V38" s="42"/>
-      <c r="W38" s="42"/>
-      <c r="X38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI38" s="43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="N38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="O38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="P38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="R38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="S38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="T38" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="U38" s="49"/>
+      <c r="V38" s="49"/>
+      <c r="W38" s="49"/>
+      <c r="X38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI38" s="49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="12" t="s">
         <v>86</v>
       </c>
@@ -4526,7 +4465,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" s="14" t="n">
         <v>0</v>
@@ -4535,88 +4474,88 @@
         <v>0</v>
       </c>
       <c r="J39" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L39" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="M39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="N39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="O39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="P39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="R39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="S39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="T39" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="U39" s="14"/>
-      <c r="V39" s="14"/>
-      <c r="W39" s="14"/>
-      <c r="X39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI39" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+      <c r="L39" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="M39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="N39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="O39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="P39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="R39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="S39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="T39" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="U39" s="49"/>
+      <c r="V39" s="49"/>
+      <c r="W39" s="49"/>
+      <c r="X39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH39" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI39" s="49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="s">
         <v>86</v>
       </c>
       <c r="B40" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="12" t="s">
-        <v>98</v>
-      </c>
       <c r="D40" s="13" t="n">
         <v>1</v>
       </c>
@@ -4627,97 +4566,97 @@
         <v>0</v>
       </c>
       <c r="G40" s="13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" s="14" t="n">
         <v>0</v>
       </c>
       <c r="I40" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K40" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="L40" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="M40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="N40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="O40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="P40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="R40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="S40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="T40" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="U40" s="14"/>
-      <c r="V40" s="14"/>
-      <c r="W40" s="14"/>
-      <c r="X40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI40" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="L40" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="M40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="N40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="O40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="P40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="R40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="S40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="T40" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="U40" s="49"/>
+      <c r="V40" s="49"/>
+      <c r="W40" s="49"/>
+      <c r="X40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI40" s="49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="s">
         <v>86</v>
       </c>
       <c r="B41" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="12" t="s">
-        <v>100</v>
-      </c>
       <c r="D41" s="13" t="n">
         <v>1</v>
       </c>
@@ -4728,499 +4667,293 @@
         <v>0</v>
       </c>
       <c r="G41" s="13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" s="14" t="n">
         <v>0</v>
       </c>
       <c r="I41" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" s="14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="M41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="N41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="O41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="P41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="R41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="S41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="T41" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="U41" s="14"/>
-      <c r="V41" s="14"/>
-      <c r="W41" s="14"/>
-      <c r="X41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI41" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+      <c r="L41" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="M41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="N41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="O41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="P41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="R41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="S41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="T41" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="U41" s="49"/>
+      <c r="V41" s="49"/>
+      <c r="W41" s="49"/>
+      <c r="X41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH41" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI41" s="49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="55" t="s">
+      <c r="B42" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="D42" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J42" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="K42" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="M42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="N42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="O42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="P42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="R42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="S42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="T42" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="U42" s="49"/>
+      <c r="V42" s="49"/>
+      <c r="W42" s="49"/>
+      <c r="X42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH42" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI42" s="49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D42" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E42" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="F42" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G42" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H42" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="K42" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="L42" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="M42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="N42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="O42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="P42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="R42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="S42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="T42" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="U42" s="14"/>
-      <c r="V42" s="14"/>
-      <c r="W42" s="14"/>
-      <c r="X42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI42" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B43" s="12" t="s">
+      <c r="C43" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D43" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E43" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="F43" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G43" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H43" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="J43" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K43" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L43" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="M43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="N43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="O43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="P43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="R43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="S43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="T43" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="U43" s="14"/>
-      <c r="V43" s="14"/>
-      <c r="W43" s="14"/>
-      <c r="X43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI43" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D44" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E44" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="F44" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H44" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="J44" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K44" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="L44" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="M44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="N44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="O44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="P44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="R44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="S44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="T44" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="U44" s="14"/>
-      <c r="V44" s="14"/>
-      <c r="W44" s="14"/>
-      <c r="X44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI44" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="D45" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="E45" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F45" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="H45" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="J45" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="K45" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="L45" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="M45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="N45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="O45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="P45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="R45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="S45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="T45" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="U45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="V45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="W45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="X45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH45" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI45" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
+      <c r="D43" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J43" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K43" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="L43" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="M43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="N43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="O43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="P43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="R43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="S43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="T43" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="U43" s="49"/>
+      <c r="V43" s="49"/>
+      <c r="W43" s="49"/>
+      <c r="X43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH43" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI43" s="49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="76">
+  <mergeCells count="80">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="P6:S6"/>
@@ -5293,10 +5026,14 @@
     <mergeCell ref="T34:W34"/>
     <mergeCell ref="L35:O35"/>
     <mergeCell ref="T35:W35"/>
-    <mergeCell ref="L36:O36"/>
-    <mergeCell ref="T36:W36"/>
-    <mergeCell ref="L38:O38"/>
-    <mergeCell ref="T38:W38"/>
+    <mergeCell ref="L36:AI36"/>
+    <mergeCell ref="L37:AI37"/>
+    <mergeCell ref="L38:AI38"/>
+    <mergeCell ref="L39:AI39"/>
+    <mergeCell ref="L40:AI40"/>
+    <mergeCell ref="L41:AI41"/>
+    <mergeCell ref="L42:AI42"/>
+    <mergeCell ref="L43:AI43"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5316,7 +5053,7 @@
   <dimension ref="A1:AG11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z11" activeCellId="1" sqref="C42:K43 Z11"/>
+      <selection pane="topLeft" activeCell="Z11" activeCellId="0" sqref="Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5329,7 +5066,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -5337,106 +5074,106 @@
       <c r="E1" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="56" t="n">
+      <c r="B3" s="50" t="n">
         <v>31</v>
       </c>
-      <c r="C3" s="56" t="n">
+      <c r="C3" s="50" t="n">
         <v>30</v>
       </c>
-      <c r="D3" s="56" t="n">
+      <c r="D3" s="50" t="n">
         <v>29</v>
       </c>
-      <c r="E3" s="56" t="n">
+      <c r="E3" s="50" t="n">
         <v>28</v>
       </c>
-      <c r="F3" s="56" t="n">
+      <c r="F3" s="50" t="n">
         <v>27</v>
       </c>
-      <c r="G3" s="56" t="n">
+      <c r="G3" s="50" t="n">
         <v>26</v>
       </c>
-      <c r="H3" s="56" t="n">
+      <c r="H3" s="50" t="n">
         <v>25</v>
       </c>
-      <c r="I3" s="56" t="n">
+      <c r="I3" s="50" t="n">
         <v>24</v>
       </c>
-      <c r="J3" s="56" t="n">
+      <c r="J3" s="50" t="n">
         <v>23</v>
       </c>
-      <c r="K3" s="56" t="n">
+      <c r="K3" s="50" t="n">
         <v>22</v>
       </c>
-      <c r="L3" s="56" t="n">
+      <c r="L3" s="50" t="n">
         <v>21</v>
       </c>
-      <c r="M3" s="56" t="n">
+      <c r="M3" s="50" t="n">
         <v>20</v>
       </c>
-      <c r="N3" s="56" t="n">
+      <c r="N3" s="50" t="n">
         <v>19</v>
       </c>
-      <c r="O3" s="56" t="n">
+      <c r="O3" s="50" t="n">
         <v>18</v>
       </c>
-      <c r="P3" s="56" t="n">
+      <c r="P3" s="50" t="n">
         <v>17</v>
       </c>
-      <c r="Q3" s="56" t="n">
+      <c r="Q3" s="50" t="n">
         <v>16</v>
       </c>
-      <c r="R3" s="56" t="n">
+      <c r="R3" s="50" t="n">
         <v>15</v>
       </c>
-      <c r="S3" s="56" t="n">
+      <c r="S3" s="50" t="n">
         <v>14</v>
       </c>
-      <c r="T3" s="56" t="n">
+      <c r="T3" s="50" t="n">
         <v>13</v>
       </c>
-      <c r="U3" s="56" t="n">
+      <c r="U3" s="50" t="n">
         <v>12</v>
       </c>
-      <c r="V3" s="56" t="n">
+      <c r="V3" s="50" t="n">
         <v>11</v>
       </c>
-      <c r="W3" s="56" t="n">
+      <c r="W3" s="50" t="n">
         <v>10</v>
       </c>
-      <c r="X3" s="56" t="n">
+      <c r="X3" s="50" t="n">
         <v>9</v>
       </c>
-      <c r="Y3" s="56" t="n">
+      <c r="Y3" s="50" t="n">
         <v>8</v>
       </c>
-      <c r="Z3" s="56" t="n">
-        <v>7</v>
-      </c>
-      <c r="AA3" s="56" t="n">
+      <c r="Z3" s="50" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA3" s="50" t="n">
         <v>6</v>
       </c>
-      <c r="AB3" s="56" t="n">
+      <c r="AB3" s="50" t="n">
         <v>5</v>
       </c>
-      <c r="AC3" s="56" t="n">
+      <c r="AC3" s="50" t="n">
         <v>4</v>
       </c>
-      <c r="AD3" s="56" t="n">
+      <c r="AD3" s="50" t="n">
         <v>3</v>
       </c>
-      <c r="AE3" s="56" t="n">
+      <c r="AE3" s="50" t="n">
         <v>2</v>
       </c>
-      <c r="AF3" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="56" t="n">
+      <c r="AF3" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="50" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AG4" s="0" t="n">
         <v>1</v>
@@ -5444,7 +5181,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AF5" s="0" t="n">
         <v>1</v>
@@ -5452,7 +5189,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="AE6" s="0" t="n">
         <v>1</v>
@@ -5460,7 +5197,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="AD7" s="0" t="n">
         <v>1</v>
@@ -5468,7 +5205,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="AC8" s="0" t="n">
         <v>1</v>
@@ -5476,7 +5213,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="AB9" s="0" t="n">
         <v>1</v>
@@ -5484,7 +5221,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="AA10" s="0" t="n">
         <v>1</v>
@@ -5492,7 +5229,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="Z11" s="0" t="n">
         <v>1</v>
@@ -5520,7 +5257,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="C42:K43 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5537,129 +5274,129 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="51" t="s">
         <v>119</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>121</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>123</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="B3" s="57" t="n">
+        <v>120</v>
+      </c>
+      <c r="B3" s="51" t="n">
         <v>54</v>
       </c>
-      <c r="C3" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="57" t="s">
-        <v>126</v>
+      <c r="C3" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="57" t="n">
+      <c r="B4" s="51" t="n">
         <v>189</v>
       </c>
-      <c r="C4" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="57" t="n">
+      <c r="C4" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5" s="57" t="n">
+        <v>122</v>
+      </c>
+      <c r="B5" s="51" t="n">
         <v>594</v>
       </c>
-      <c r="C5" s="57" t="n">
+      <c r="C5" s="51" t="n">
         <v>416</v>
       </c>
-      <c r="D5" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="57" t="n">
+      <c r="D5" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="57" t="n">
+        <v>123</v>
+      </c>
+      <c r="B6" s="51" t="n">
         <v>321</v>
       </c>
-      <c r="C6" s="57" t="n">
+      <c r="C6" s="51" t="n">
         <v>416</v>
       </c>
-      <c r="D6" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="57" t="n">
+      <c r="D6" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="n">

</xml_diff>

<commit_message>
Hello, World! Runs on the R32V2020
</commit_message>
<xml_diff>
--- a/Architecture/OpCodes/R32V2020.xlsx
+++ b/Architecture/OpCodes/R32V2020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="OpCodes" sheetId="1" state="visible" r:id="rId2"/>
@@ -2229,7 +2229,7 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AA11" activeCellId="0" sqref="AA11"/>
     </sheetView>
   </sheetViews>
@@ -6331,14 +6331,14 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="3" style="0" width="3.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="25" style="0" width="2.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="3.79"/>
@@ -7369,7 +7369,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.3"/>

</xml_diff>